<commit_message>
update read filepath to rankdata
</commit_message>
<xml_diff>
--- a/ExpertData/1_ExportScoreData.xlsx
+++ b/ExpertData/1_ExportScoreData.xlsx
@@ -159,7 +159,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2"/>
+      <c r="C2" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
@@ -171,7 +173,9 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3"/>
+      <c r="C3" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
@@ -183,7 +187,9 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4"/>
+      <c r="C4" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
@@ -195,7 +201,9 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5"/>
+      <c r="C5" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
@@ -207,7 +215,9 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6"/>
+      <c r="C6" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
@@ -219,7 +229,9 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7"/>
+      <c r="C7" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
@@ -231,7 +243,9 @@
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8"/>
+      <c r="C8" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
@@ -243,7 +257,9 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9"/>
+      <c r="C9" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
@@ -255,7 +271,9 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10"/>
+      <c r="C10" s="2">
+        <v>0.01</v>
+      </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>

</xml_diff>